<commit_message>
Added few functions and core mechanics
</commit_message>
<xml_diff>
--- a/dataBase/humanAncestry.xlsx
+++ b/dataBase/humanAncestry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projecs\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67067D0-8AD9-48E1-8081-81BC533B733D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA72784-F020-42B2-8661-05FAD1E415AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="10530" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ludzie" sheetId="1" r:id="rId1"/>
@@ -31,54 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
-  <si>
-    <t>Siła</t>
-  </si>
-  <si>
-    <t>Zręczność</t>
-  </si>
-  <si>
-    <t>Intelekt</t>
-  </si>
-  <si>
-    <t>Wola</t>
-  </si>
-  <si>
-    <t>Percepcja</t>
-  </si>
-  <si>
-    <t>Zdrowie</t>
-  </si>
-  <si>
-    <t>Szybkość Zdrowienia</t>
-  </si>
-  <si>
-    <t>Rozmiar</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
   <si>
     <t>0.5</t>
-  </si>
-  <si>
-    <t>Prędkość</t>
-  </si>
-  <si>
-    <t>Moc</t>
-  </si>
-  <si>
-    <t>Obrażenia</t>
-  </si>
-  <si>
-    <t>Szaleństwo</t>
-  </si>
-  <si>
-    <t>Splugawienie</t>
-  </si>
-  <si>
-    <t>Język Mowa</t>
-  </si>
-  <si>
-    <t>Język Pismo</t>
   </si>
   <si>
     <t>Wspólny</t>
@@ -240,9 +195,6 @@
   </si>
   <si>
     <t>Jesteś wysoki i szczupły.</t>
-  </si>
-  <si>
-    <t>Jesteś bardzo wysoki i masywny</t>
   </si>
   <si>
     <t>Jesteś szpetny. Wyglądasz jak maszkara. Dzieci płaczą
@@ -285,14 +237,116 @@
 że ta osoba zwróci się przeciw tobie.</t>
   </si>
   <si>
-    <t>Obrona</t>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Siła:</t>
+  </si>
+  <si>
+    <t>Zręczność:</t>
+  </si>
+  <si>
+    <t>Intelekt:</t>
+  </si>
+  <si>
+    <t>Wola:</t>
+  </si>
+  <si>
+    <t>Percepcja:</t>
+  </si>
+  <si>
+    <t>Zdrowie:</t>
+  </si>
+  <si>
+    <t>Szybkość Zdrowienia:</t>
+  </si>
+  <si>
+    <t>Rozmiar:</t>
+  </si>
+  <si>
+    <t>Prędkość:</t>
+  </si>
+  <si>
+    <t>Obrona:</t>
+  </si>
+  <si>
+    <t>Moc:</t>
+  </si>
+  <si>
+    <t>Obrażenia:</t>
+  </si>
+  <si>
+    <t>Szaleństwo:</t>
+  </si>
+  <si>
+    <t>Splugawienie:</t>
+  </si>
+  <si>
+    <t>Język Mowa:</t>
+  </si>
+  <si>
+    <t>Język Pismo:</t>
+  </si>
+  <si>
+    <t>wybór rozmiaru</t>
+  </si>
+  <si>
+    <t>16-18</t>
+  </si>
+  <si>
+    <t>5-6</t>
+  </si>
+  <si>
+    <t>7-10</t>
+  </si>
+  <si>
+    <t>11-15</t>
+  </si>
+  <si>
+    <t>4-7</t>
+  </si>
+  <si>
+    <t>8-12</t>
+  </si>
+  <si>
+    <t>13-15</t>
+  </si>
+  <si>
+    <t>16-17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>7-8</t>
+  </si>
+  <si>
+    <t>9-12</t>
+  </si>
+  <si>
+    <t>13-14</t>
+  </si>
+  <si>
+    <t>15-16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Jesteś bardzo wysoki i masywny.</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,9 +355,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Metropolis-Regular"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -326,14 +408,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -614,28 +722,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>10</v>
+      <c r="A1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -643,37 +752,40 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -681,26 +793,23 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -708,15 +817,15 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -724,7 +833,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -732,7 +841,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -740,7 +849,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -748,15 +857,26 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -767,115 +887,184 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1C835C-BECA-4F8C-A233-A9EE9639DEEB}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="78.7109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -885,60 +1074,96 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8480B0-5918-48AA-B46C-6EB33A4C5A54}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>47</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -949,87 +1174,148 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C1A233-0509-402B-B85D-4518C9CFAD27}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" style="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>53</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>3</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>4</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C11F06-6C34-4B96-A0EB-8272E8FEDC76}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>59</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1039,57 +1325,96 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667A7402-EBD6-4409-993E-3F477E26BC07}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="30.42578125" style="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>68</v>
+      <c r="B1" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1099,61 +1424,97 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0FC315-B645-4D42-9588-47C4BDCA9461}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>71</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>3</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>4</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>77</v>
+      <c r="A4" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
passing ancestry to data base picker
</commit_message>
<xml_diff>
--- a/dataBase/humanAncestry.xlsx
+++ b/dataBase/humanAncestry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projecs\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA72784-F020-42B2-8661-05FAD1E415AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914C944B-26EA-4FD1-9DF4-AE27FA469EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="10530" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ludzie" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Budowa Ciała" sheetId="7" r:id="rId6"/>
     <sheet name="Wygląd" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,9 +39,6 @@
     <t>Wspólny</t>
   </si>
   <si>
-    <t>Zwiekszenie dowolnego atrybutu o 1</t>
-  </si>
-  <si>
     <t>Wybór dodatkowego języka lub losowej profesji</t>
   </si>
   <si>
@@ -291,9 +288,6 @@
     <t>Język Pismo:</t>
   </si>
   <si>
-    <t>wybór rozmiaru</t>
-  </si>
-  <si>
     <t>16-18</t>
   </si>
   <si>
@@ -340,6 +334,12 @@
   </si>
   <si>
     <t>result</t>
+  </si>
+  <si>
+    <t>Czytanie i pisanie wspólny</t>
+  </si>
+  <si>
+    <t>2k6 miedziaków</t>
   </si>
 </sst>
 </file>
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,15 +736,15 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -752,40 +752,34 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -793,7 +787,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -801,7 +795,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -809,7 +803,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -817,7 +811,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -825,7 +819,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -833,7 +827,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -841,7 +835,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -849,7 +843,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -857,7 +851,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -865,12 +859,12 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -887,184 +881,190 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1C835C-BECA-4F8C-A233-A9EE9639DEEB}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1088,10 +1088,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1099,7 +1099,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1107,47 +1107,47 @@
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1155,7 +1155,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1176,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C1A233-0509-402B-B85D-4518C9CFAD27}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,10 +1188,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1199,7 +1199,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1207,39 +1207,39 @@
         <v>4</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1253,7 +1253,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,10 +1264,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1275,47 +1275,47 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1328,7 +1328,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,10 +1339,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1350,7 +1350,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1358,63 +1358,63 @@
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1426,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0FC315-B645-4D42-9588-47C4BDCA9461}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,10 +1438,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1449,7 +1449,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1458,63 +1458,63 @@
         <v>4</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed IF statements to `match-case`.
</commit_message>
<xml_diff>
--- a/dataBase/humanAncestry.xlsx
+++ b/dataBase/humanAncestry.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projecs\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914C944B-26EA-4FD1-9DF4-AE27FA469EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F05E62-6DC9-4D9D-9C88-F3B7E3790755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5595" yWindow="2955" windowWidth="28800" windowHeight="16515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ludzie" sheetId="1" r:id="rId1"/>
+    <sheet name="humanAncestry" sheetId="1" r:id="rId1"/>
     <sheet name="Przeszłość" sheetId="2" r:id="rId2"/>
     <sheet name="Osobowość" sheetId="3" r:id="rId3"/>
     <sheet name="Religia" sheetId="4" r:id="rId4"/>
@@ -408,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -418,17 +418,14 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -725,7 +722,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,12 +886,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" style="10" customWidth="1"/>
     <col min="2" max="2" width="90.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -902,7 +899,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -910,7 +907,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -918,7 +915,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -926,7 +923,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -934,7 +931,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -942,7 +939,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -950,7 +947,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -958,7 +955,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -966,7 +963,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -974,7 +971,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -982,7 +979,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -990,7 +987,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -998,7 +995,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1006,7 +1003,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -1017,7 +1014,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -1025,7 +1022,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1033,7 +1030,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1041,7 +1038,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="A19" s="10">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1049,7 +1046,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -1057,7 +1054,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -1082,12 +1079,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="88.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -1095,7 +1092,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1103,7 +1100,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1111,7 +1108,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1119,7 +1116,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1127,7 +1124,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1135,7 +1132,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>90</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1143,7 +1140,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1151,7 +1148,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>17</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1159,7 +1156,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1182,63 +1179,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="3">
         <v>3</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3" s="3">
         <v>4</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1258,12 +1255,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1271,7 +1268,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="3">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1279,7 +1276,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1287,7 +1284,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1295,7 +1292,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1303,7 +1300,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1311,7 +1308,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1333,12 +1330,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="30.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1346,7 +1343,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="3">
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1354,7 +1351,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="3">
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1362,7 +1359,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1370,7 +1367,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1378,7 +1375,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1386,7 +1383,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1394,7 +1391,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1402,7 +1399,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1410,7 +1407,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1432,12 +1429,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1445,75 +1442,75 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+      <c r="A2" s="13">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="13">
         <v>4</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hero object it is passed to backstory methods
</commit_message>
<xml_diff>
--- a/dataBase/humanAncestry.xlsx
+++ b/dataBase/humanAncestry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projecs\pythonProject\dataBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJEKTY\CODING\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F05E62-6DC9-4D9D-9C88-F3B7E3790755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9BAAAC-523B-4ADD-911E-EA74721E48BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="2955" windowWidth="28800" windowHeight="16515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57495" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="humanAncestry" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="102">
   <si>
     <t>0.5</t>
   </si>
@@ -340,6 +340,21 @@
   </si>
   <si>
     <t>2k6 miedziaków</t>
+  </si>
+  <si>
+    <t>1 punkt splugawienia</t>
+  </si>
+  <si>
+    <t>1 punkt szaleństwa</t>
+  </si>
+  <si>
+    <t>1k6-2 dzieci</t>
+  </si>
+  <si>
+    <t>Mówisz w dodatkowym języku</t>
+  </si>
+  <si>
+    <t>addition</t>
   </si>
 </sst>
 </file>
@@ -722,7 +737,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1C835C-BECA-4F8C-A233-A9EE9639DEEB}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,6 +912,9 @@
       <c r="B1" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
@@ -913,6 +931,9 @@
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
@@ -929,6 +950,9 @@
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
@@ -945,6 +969,9 @@
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
@@ -993,6 +1020,9 @@
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="C13" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -1000,6 +1030,9 @@
       </c>
       <c r="B14" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1250,7 +1283,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added quirks and languages choice option
</commit_message>
<xml_diff>
--- a/dataBase/humanAncestry.xlsx
+++ b/dataBase/humanAncestry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJEKTY\CODING\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C83CB18-DB9B-45D9-A5C1-43A6982566CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ED4674-FA96-4FE3-8AD7-707D1DE632E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="humanAncestry" sheetId="1" r:id="rId1"/>
@@ -740,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -899,7 +899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90C11F06-6C34-4B96-A0EB-8272E8FEDC76}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correcting data base attribute locations
</commit_message>
<xml_diff>
--- a/dataBase/humanAncestry.xlsx
+++ b/dataBase/humanAncestry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJEKTY\CODING\pythonProject\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ED4674-FA96-4FE3-8AD7-707D1DE632E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F1BD7-2062-4C8E-BDF2-4B46CB4E1141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6030" yWindow="3105" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="humanAncestry" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="101">
   <si>
     <t>0.5</t>
   </si>
   <si>
     <t>Wspólny</t>
-  </si>
-  <si>
-    <t>Wybór dodatkowego języka lub losowej profesji</t>
   </si>
   <si>
     <t>Umarłeś i powróciłeś do żywych. Zaczynasz grę z 1k6 punktów Szaleństwa.</t>
@@ -738,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,137 +747,134 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>62</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -911,10 +905,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,47 +916,47 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -986,13 +980,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1008,10 +1002,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1019,7 +1013,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,10 +1021,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1038,7 +1032,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,10 +1040,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1057,7 +1051,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1065,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1073,7 +1067,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1081,7 +1075,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,7 +1083,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1097,10 +1091,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,10 +1102,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1119,10 +1113,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1130,7 +1124,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1138,7 +1132,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1146,7 +1140,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1154,7 +1148,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1162,7 +1156,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1170,10 +1164,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1197,10 +1191,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1208,7 +1202,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1216,47 +1210,47 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1264,7 +1258,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1272,7 +1266,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1297,10 +1291,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1308,7 +1302,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1316,39 +1310,39 @@
         <v>4</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1373,10 +1367,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1384,7 +1378,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1393,63 +1387,63 @@
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1473,10 +1467,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1484,7 +1478,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1492,63 +1486,63 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>